<commit_message>
progress with jekyll. ready to test
</commit_message>
<xml_diff>
--- a/lothiancriticalcare/1a74f8f7b8b7e871b413c4697f68b4401fbacdf0/reviewdates.xlsx
+++ b/lothiancriticalcare/1a74f8f7b8b7e871b413c4697f68b4401fbacdf0/reviewdates.xlsx
@@ -67,18 +67,18 @@
     <t>Infection_and_sepsis/SARI/MERS-CoV Guideline.pdf</t>
   </si>
   <si>
+    <t>Infection_and_sepsis/SARI/Suspected Influeza A Avian influenza H5N1 and SARS.pdf</t>
+  </si>
+  <si>
     <t>Infection_and_sepsis/SARI/Suspected Influeza A-H7N9 Guideline.pdf</t>
   </si>
   <si>
-    <t>Infection_and_sepsis/SARI/Suspected Influeza A Avian influenza H5N1 and SARS.pdf</t>
+    <t>Airway/Critical care extubation checklist.pdf</t>
   </si>
   <si>
     <t>ECLS/Extra Corporeal Carbon Dioxide Removal.pdf</t>
   </si>
   <si>
-    <t>Airway/Critical care extubation checklist.pdf</t>
-  </si>
-  <si>
     <t>Airway/Tracheostomy_Laryngectomy/Hospital_in-patients_with_a_Tracheostomy.pdf</t>
   </si>
   <si>
@@ -94,15 +94,15 @@
     <t>End_of_life_care/Reasons to report a death to PF.pdf</t>
   </si>
   <si>
+    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy suctioning cleaning guideline.pdf</t>
+  </si>
+  <si>
+    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy change in Critical Care.pdf</t>
+  </si>
+  <si>
     <t>Neurological/SOP -  Femoral site care.pdf</t>
   </si>
   <si>
-    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy suctioning cleaning guideline.pdf</t>
-  </si>
-  <si>
-    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy change in Critical Care.pdf</t>
-  </si>
-  <si>
     <t>Drugs/sodium_bicarbonate.pdf</t>
   </si>
   <si>
@@ -112,24 +112,24 @@
     <t>Post_op_care/Epidural top-up.pdf</t>
   </si>
   <si>
+    <t>Covid-19/SJH/SJH COVID19 ITU Intubation Action Card.pdf</t>
+  </si>
+  <si>
+    <t>Diabetes_and_Glucose/Hyperosmolar Hyperglycaemic State.pdf</t>
+  </si>
+  <si>
+    <t>Covid-19/SJH/SJH COVID19 ED Intubation Action Card.pdf</t>
+  </si>
+  <si>
+    <t>Covid-19/WGH/CoVid intubation checklist WGH.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/heparin for Haemofiltration.pdf</t>
+  </si>
+  <si>
     <t>Airway/Emergency intubation checklist_em_pub.pdf</t>
   </si>
   <si>
-    <t>Drugs/heparin for Haemofiltration.pdf</t>
-  </si>
-  <si>
-    <t>Covid-19/WGH/CoVid intubation checklist WGH.pdf</t>
-  </si>
-  <si>
-    <t>Covid-19/SJH/SJH COVID19 ED Intubation Action Card.pdf</t>
-  </si>
-  <si>
-    <t>Covid-19/SJH/SJH COVID19 ITU Intubation Action Card.pdf</t>
-  </si>
-  <si>
-    <t>Diabetes_and_Glucose/Hyperosmolar Hyperglycaemic State.pdf</t>
-  </si>
-  <si>
     <t>Drugs/fentanyl.pdf</t>
   </si>
   <si>
@@ -148,13 +148,16 @@
     <t>Airway/Percutaneous tracheostomy checklist.pdf</t>
   </si>
   <si>
+    <t>Infection_and_sepsis/SOP Ultrasound Cleaning.pdf</t>
+  </si>
+  <si>
     <t>Delirium/Managing a Potentially Violent Patient.pdf</t>
   </si>
   <si>
     <t>Delirium/Risk assessment posi mit.pdf</t>
   </si>
   <si>
-    <t>Infection_and_sepsis/SOP Ultrasound Cleaning.pdf</t>
+    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy safety box contents.pdf</t>
   </si>
   <si>
     <t>Delirium/Drugs Causing Delirium and Agitiation.pdf</t>
@@ -163,48 +166,45 @@
     <t>GI_Liver_and_Transplant/Treatment of constipation.pdf</t>
   </si>
   <si>
+    <t>Breathing(Respiratory)/HFNO.pdf</t>
+  </si>
+  <si>
     <t>GI_Liver_and_Transplant/Abdominal pressure measurement.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/HFNO.pdf</t>
+    <t>Neurological/Sub arachnoid haemorrhage management.pdf</t>
+  </si>
+  <si>
+    <t>Airway/Anticipated difficult airway tool.pdf</t>
+  </si>
+  <si>
+    <t>Airway/McGrath Mac.pdf</t>
   </si>
   <si>
     <t>Drugs/ketamine_in_asthma.pdf</t>
   </si>
   <si>
-    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy safety box contents.pdf</t>
-  </si>
-  <si>
-    <t>Neurological/Sub arachnoid haemorrhage management.pdf</t>
-  </si>
-  <si>
-    <t>Airway/Anticipated difficult airway tool.pdf</t>
-  </si>
-  <si>
-    <t>Airway/McGrath Mac.pdf</t>
-  </si>
-  <si>
     <t>End_of_life_care/Documentation following death.pdf</t>
   </si>
   <si>
+    <t>Drugs/zanamivir.pdf</t>
+  </si>
+  <si>
     <t>GI_Liver_and_Transplant/stress ulcer prophylaxis.pdf</t>
   </si>
   <si>
-    <t>Drugs/zanamivir.pdf</t>
-  </si>
-  <si>
     <t>Routine_Care/bBraun Spaceplus Failure EMERGENCY ACTION CARD_em.pdf</t>
   </si>
   <si>
     <t>Drugs/phosphate.pdf</t>
   </si>
   <si>
+    <t>Drugs/insulin.pdf</t>
+  </si>
+  <si>
     <t>Breathing(Respiratory)/Equipment/HFNO Set Up.pdf</t>
   </si>
   <si>
-    <t>Drugs/insulin.pdf</t>
-  </si>
-  <si>
     <t>Breathing(Respiratory)/Inhaled Nitrous Oxide.pdf</t>
   </si>
   <si>
@@ -217,12 +217,12 @@
     <t>Post_op_care/Epidural Haematoma.pdf</t>
   </si>
   <si>
+    <t>Breathing(Respiratory)/Equipment/T piece Y piece.pdf</t>
+  </si>
+  <si>
     <t>Neurological/SOP for review of Neurosurgical patients in ITU by neurosurgical team.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/Equipment/T piece Y piece.pdf</t>
-  </si>
-  <si>
     <t>Policies_and_admin/General Critical Care Interaction with HEPMA_pub.pdf</t>
   </si>
   <si>
@@ -253,133 +253,196 @@
     <t>GI_Liver_and_Transplant/Nasogastric feeding protocol.pdf</t>
   </si>
   <si>
+    <t>Drugs/Antibiotic doses in CVVHD.pdf</t>
+  </si>
+  <si>
+    <t>Diabetes_and_Glucose/Intravenous Insulin Therapy (not for DKA or HHS).pdf</t>
+  </si>
+  <si>
+    <t>Drugs/calcium.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/Jejunostomy feeding protocol.pdf</t>
+  </si>
+  <si>
+    <t>ECLS/RIE ECLS Anti Xa Protocol.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/Nasojejunal feeding protocol.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/vasopressin organ donation.pdf</t>
+  </si>
+  <si>
+    <t>Infection_and_sepsis/Winter Infections Stepdown Guidance.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/vasopressin_sepsis.pdf</t>
+  </si>
+  <si>
+    <t>Transfer/ACCP Transfers.pdf</t>
+  </si>
+  <si>
+    <t>Covid-19/videos/Donning and Doffing Video.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/valproate.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/thiopentone.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/ketamine for status epilepticus.pdf</t>
+  </si>
+  <si>
+    <t>Breathing(Respiratory)/Equipment/Ventilators Circuits Filters and Closed Suction - Set up and Maintenance.pdf</t>
+  </si>
+  <si>
+    <t>Breathing(Respiratory)/CPAP.pdf</t>
+  </si>
+  <si>
+    <t>Breathing(Respiratory)/Equipment/Bipap V60.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/piperacillin_tazobactam extended_infusion.pdf</t>
+  </si>
+  <si>
+    <t>Infection_and_sepsis/Infection indications for IVIG.pdf</t>
+  </si>
+  <si>
+    <t>Covid-19/Covid 19 Death Certification Guideline.pdf</t>
+  </si>
+  <si>
+    <t>Procedures/CVC Guidance/Securing CVCs.pdf</t>
+  </si>
+  <si>
+    <t>Routine_Care/Video Communication.pdf</t>
+  </si>
+  <si>
+    <t>Neurological/Treatment of status epilepticus.pdf</t>
+  </si>
+  <si>
+    <t>Cardiovascular/Cardiogenic Shock.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/isoprenaline.pdf</t>
+  </si>
+  <si>
+    <t>Haematology_CAR-T/Haem_ICU_transfer.pdf</t>
+  </si>
+  <si>
     <t>Infection_and_sepsis/SARI/Influenza A and B Virology Sampling and Oseltamivir Dose.pdf</t>
   </si>
   <si>
-    <t>Diabetes_and_Glucose/Intravenous Insulin Therapy (not for DKA or HHS).pdf</t>
-  </si>
-  <si>
-    <t>Drugs/Antibiotic doses in CVVHD.pdf</t>
+    <t>Drugs/aminophylline.pdf</t>
+  </si>
+  <si>
+    <t>Cardiovascular/Management of hypertension within Critical Care.pdf</t>
   </si>
   <si>
     <t>Cardiovascular/Central Venous Catheters - Guideline for Management of Misplacement.pdf</t>
   </si>
   <si>
+    <t>Haematology_CAR-T/CRS.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/phenytoin.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/rocuronium.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/pancuronium.pdf</t>
+  </si>
+  <si>
+    <t>Haematology_CAR-T/ICANS.pdf</t>
+  </si>
+  <si>
     <t>Drugs/nimodipine.pdf</t>
   </si>
   <si>
-    <t>Drugs/calcium.pdf</t>
-  </si>
-  <si>
-    <t>ECLS/RIE ECLS Anti Xa Protocol.pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/Nasojejunal feeding protocol.pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/Jejunostomy feeding protocol.pdf</t>
+    <t>Policies_and_admin/General Critical Care SOP_pub.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/milrinone.pdf</t>
+  </si>
+  <si>
+    <t>Organ_donation/Organ Retrieval SOP.pdf</t>
+  </si>
+  <si>
+    <t>End_of_life_care/Withdrawal of invasive ventilation nursing guide MJB 050623-1.pdf</t>
+  </si>
+  <si>
+    <t>Infection_and_sepsis/Trip Out of Unit infection guidance.pdf</t>
+  </si>
+  <si>
+    <t>End_of_life_care/CMO &amp; NRS Guidance for Doctors completing MCCD - Sept 22.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/clonidine.pdf</t>
+  </si>
+  <si>
+    <t>Covid-19/COVID 19 ICM guidance basic goals_June_2022.pdf</t>
+  </si>
+  <si>
+    <t>Neurological/Management of traumatic brain injury.pdf</t>
   </si>
   <si>
     <t>Ethics_and_Law/Care at the End of Life (FICM).pdf</t>
   </si>
   <si>
-    <t>Drugs/vasopressin_sepsis.pdf</t>
+    <t>Ethics_and_Law/DNACPR policy for Scotland.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/ICU - Upper GI bleeding (Endoscopy guideline).pdf</t>
   </si>
   <si>
     <t>Neurological/Critical Care MRI Procedure_pub.pdf</t>
   </si>
   <si>
-    <t>End_of_life_care/CMO &amp; NRS Guidance for Doctors completing MCCD - Sept 22.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/vasopressin organ donation.pdf</t>
-  </si>
-  <si>
-    <t>Neurological/Management of traumatic brain injury.pdf</t>
-  </si>
-  <si>
-    <t>Ethics_and_Law/DNACPR policy for Scotland.pdf</t>
-  </si>
-  <si>
-    <t>Covid-19/COVID 19 ICM guidance basic goals_June_2022.pdf</t>
-  </si>
-  <si>
-    <t>Organ_donation/Organ Retrieval SOP.pdf</t>
-  </si>
-  <si>
-    <t>Infection_and_sepsis/Winter Infections Stepdown Guidance.pdf</t>
-  </si>
-  <si>
-    <t>Infection_and_sepsis/Trip Out of Unit infection guidance.pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/ICU - Upper GI bleeding (Endoscopy guideline).pdf</t>
-  </si>
-  <si>
     <t>Airway/Cook Staged Extubation Set.pdf</t>
   </si>
   <si>
-    <t>Drugs/ketamine for status epilepticus.pdf</t>
-  </si>
-  <si>
-    <t>Covid-19/videos/Donning and Doffing Video.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/thiopentone.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/valproate.pdf</t>
-  </si>
-  <si>
-    <t>End_of_life_care/Withdrawal of invasive ventilation nursing guide MJB 050623-1.pdf</t>
-  </si>
-  <si>
-    <t>Transfer/ACCP Transfers.pdf</t>
-  </si>
-  <si>
     <t>End_of_life_care/Draft NHS Lothian Critical Care End of Life care Guidance Edited June 24th 2023 MIB 050623 (1)-1.pdf</t>
   </si>
   <si>
+    <t>Drugs/noradrenaline (central).pdf</t>
+  </si>
+  <si>
     <t>Post_op_care/Epidural hypotension.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/Equipment/Bipap V60.pdf</t>
-  </si>
-  <si>
-    <t>Breathing(Respiratory)/Equipment/Ventilators Circuits Filters and Closed Suction - Set up and Maintenance.pdf</t>
-  </si>
-  <si>
-    <t>Infection_and_sepsis/Infection indications for IVIG.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/piperacillin_tazobactam extended_infusion.pdf</t>
-  </si>
-  <si>
-    <t>Breathing(Respiratory)/CPAP.pdf</t>
+    <t>Drugs/dexmedetomidine.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/glyceryl_trinitrate.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/Fulminant Liver Failure.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/Confirmation of Nasogastric Tube Position.pdf</t>
+  </si>
+  <si>
+    <t>Breathing(Respiratory)/Equipment/Passy Muir Valve.pdf</t>
   </si>
   <si>
     <t>Transfer/Transfer Outdoors to Garden Guideline.pdf</t>
   </si>
   <si>
-    <t>Covid-19/Covid 19 Death Certification Guideline.pdf</t>
-  </si>
-  <si>
-    <t>Procedures/CVC Guidance/Securing CVCs.pdf</t>
+    <t>Cardiovascular/Intra Aortic Balloon Pump Guideline_pub.pdf</t>
+  </si>
+  <si>
+    <t>Cardiovascular/Intra Aortic Balloon Pump Bedside Checks_pub.pdf</t>
   </si>
   <si>
     <t>Breathing(Respiratory)/ARDS Strategy.pdf</t>
   </si>
   <si>
-    <t>Neurological/Treatment of status epilepticus.pdf</t>
-  </si>
-  <si>
-    <t>Routine_Care/Video Communication.pdf</t>
-  </si>
-  <si>
-    <t>Cardiovascular/Cardiogenic Shock.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/isoprenaline.pdf</t>
+    <t>Drugs/dobutamine.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/adrenaline.pdf</t>
   </si>
   <si>
     <t>Drugs/hydralazine.pdf</t>
@@ -394,73 +457,16 @@
     <t>Drugs/magnesium.pdf</t>
   </si>
   <si>
-    <t>Haematology_CAR-T/Haem_ICU_transfer.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/aminophylline.pdf</t>
-  </si>
-  <si>
-    <t>Cardiovascular/Management of hypertension within Critical Care.pdf</t>
-  </si>
-  <si>
-    <t>Haematology_CAR-T/CRS.pdf</t>
-  </si>
-  <si>
-    <t>Haematology_CAR-T/ICANS.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/pancuronium.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/phenytoin.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/rocuronium.pdf</t>
-  </si>
-  <si>
-    <t>Policies_and_admin/General Critical Care SOP_pub.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/milrinone.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/clonidine.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/noradrenaline (central).pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/Confirmation of Nasogastric Tube Position.pdf</t>
-  </si>
-  <si>
-    <t>Breathing(Respiratory)/Equipment/Passy Muir Valve.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/glyceryl_trinitrate.pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/Fulminant Liver Failure.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/dexmedetomidine.pdf</t>
-  </si>
-  <si>
-    <t>Cardiovascular/Intra Aortic Balloon Pump Guideline_pub.pdf</t>
-  </si>
-  <si>
-    <t>Cardiovascular/Intra Aortic Balloon Pump Bedside Checks_pub.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/dobutamine.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/adrenaline.pdf</t>
+    <t>Drugs/neostigmine.pdf</t>
   </si>
   <si>
     <t>Drugs/vancomycin.pdf</t>
   </si>
   <si>
-    <t>Drugs/neostigmine.pdf</t>
+    <t>Drugs/labetalol.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/alteplase for massive PE.pdf</t>
   </si>
   <si>
     <t>Infection_and_sepsis/Initial investigation and management in unidentified Infections.pdf</t>
@@ -469,60 +475,54 @@
     <t>Neurological/Intrathecal policy RIE feb 2023.1.pdf</t>
   </si>
   <si>
-    <t>Drugs/labetalol.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/alteplase for massive PE.pdf</t>
-  </si>
-  <si>
     <t>Cardiovascular/Management of Acute Type B Aortic Dissection Guideline.pdf</t>
   </si>
   <si>
     <t>Drugs/midazolam.pdf</t>
   </si>
   <si>
+    <t>Procedures/CVC Guidance/CVC NHL  April 2023.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/potassium.pdf</t>
+  </si>
+  <si>
     <t>Drugs/salbutamol.pdf</t>
   </si>
   <si>
-    <t>Drugs/potassium.pdf</t>
-  </si>
-  <si>
-    <t>Procedures/CVC Guidance/CVC NHL  April 2023.pdf</t>
+    <t>Procedures/Arterial Line insertion for ACCPs.pdf</t>
   </si>
   <si>
     <t>Drugs/amiodarone.pdf</t>
   </si>
   <si>
-    <t>Procedures/Arterial Line insertion for ACCPs.pdf</t>
+    <t>Routine_Care/ICU Eye Care Guideline.pdf</t>
   </si>
   <si>
     <t>Drugs/nicardipine.pdf</t>
   </si>
   <si>
-    <t>Routine_Care/ICU Eye Care Guideline.pdf</t>
-  </si>
-  <si>
     <t>Drugs/phenobarbitone.pdf</t>
   </si>
   <si>
+    <t>Drugs/noradrenaline (peripheral).pdf</t>
+  </si>
+  <si>
     <t>Breathing(Respiratory)/Manual Ventilation and MHI.pdf</t>
   </si>
   <si>
+    <t>Drugs/Epoprostenol.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/Morphine 2023 v3.pdf</t>
+  </si>
+  <si>
     <t>Neurological/Ventriculitis Guideline.pdf</t>
   </si>
   <si>
-    <t>Drugs/Epoprostenol.pdf</t>
-  </si>
-  <si>
     <t>Drugs/Phenylephrine v4 Jun 2023.pdf</t>
   </si>
   <si>
-    <t>Drugs/noradrenaline (peripheral).pdf</t>
-  </si>
-  <si>
-    <t>Drugs/Morphine 2023 v3.pdf</t>
-  </si>
-  <si>
     <t>Cardiovascular/Cardiac Output Monitoring_pub .pdf</t>
   </si>
   <si>
@@ -538,15 +538,15 @@
     <t>Breathing(Respiratory)/Proning Guideline.pdf</t>
   </si>
   <si>
+    <t>Post_op_care/Prevention and treatment of paraplegia after major aortic procedures.pdf</t>
+  </si>
+  <si>
     <t>Procedures/ACCPs acquiring initial CVC competencies.pdf</t>
   </si>
   <si>
     <t>Procedures/ACCP CVC placement following completion of initial competencies.pdf</t>
   </si>
   <si>
-    <t>Post_op_care/Prevention and treatment of paraplegia after major aortic procedures.pdf</t>
-  </si>
-  <si>
     <t>Breathing(Respiratory)/Equipment/NIV Set up in Critical Care.pdf</t>
   </si>
   <si>
@@ -556,268 +556,268 @@
     <t>Post_op_care/Perioperative Care of the Transgender or Non-Binary Pateint.pdf</t>
   </si>
   <si>
-    <t>2011-03-10</t>
-  </si>
-  <si>
-    <t>2011-06-10</t>
-  </si>
-  <si>
-    <t>2011-07-10</t>
-  </si>
-  <si>
-    <t>2011-12-10</t>
-  </si>
-  <si>
-    <t>2014-09-10</t>
-  </si>
-  <si>
-    <t>2014-10-10</t>
-  </si>
-  <si>
-    <t>2014-11-10</t>
-  </si>
-  <si>
-    <t>2014-12-10</t>
-  </si>
-  <si>
-    <t>2015-03-10</t>
-  </si>
-  <si>
-    <t>2016-01-10</t>
-  </si>
-  <si>
-    <t>2016-04-10</t>
-  </si>
-  <si>
-    <t>2016-08-10</t>
-  </si>
-  <si>
-    <t>2017-01-10</t>
-  </si>
-  <si>
-    <t>2017-08-10</t>
-  </si>
-  <si>
-    <t>2017-09-10</t>
-  </si>
-  <si>
-    <t>2017-10-10</t>
-  </si>
-  <si>
-    <t>2017-11-10</t>
-  </si>
-  <si>
-    <t>2018-05-10</t>
-  </si>
-  <si>
-    <t>2018-07-10</t>
-  </si>
-  <si>
-    <t>2019-05-10</t>
-  </si>
-  <si>
-    <t>2019-06-10</t>
-  </si>
-  <si>
-    <t>2019-08-10</t>
-  </si>
-  <si>
-    <t>2019-09-10</t>
-  </si>
-  <si>
-    <t>2020-01-10</t>
-  </si>
-  <si>
-    <t>2020-03-10</t>
-  </si>
-  <si>
-    <t>2020-04-10</t>
-  </si>
-  <si>
-    <t>2020-05-10</t>
-  </si>
-  <si>
-    <t>2020-07-10</t>
-  </si>
-  <si>
-    <t>2020-08-10</t>
-  </si>
-  <si>
-    <t>2020-11-10</t>
-  </si>
-  <si>
-    <t>2021-02-10</t>
-  </si>
-  <si>
-    <t>2021-05-10</t>
-  </si>
-  <si>
-    <t>2021-06-10</t>
-  </si>
-  <si>
-    <t>2021-09-10</t>
-  </si>
-  <si>
-    <t>2021-12-10</t>
-  </si>
-  <si>
-    <t>2022-01-10</t>
-  </si>
-  <si>
-    <t>2022-03-10</t>
-  </si>
-  <si>
-    <t>2022-04-10</t>
-  </si>
-  <si>
-    <t>2022-05-10</t>
-  </si>
-  <si>
-    <t>2022-06-10</t>
-  </si>
-  <si>
-    <t>2022-07-10</t>
-  </si>
-  <si>
-    <t>2022-08-10</t>
-  </si>
-  <si>
-    <t>2022-09-10</t>
-  </si>
-  <si>
-    <t>2022-10-10</t>
-  </si>
-  <si>
-    <t>2022-11-10</t>
-  </si>
-  <si>
-    <t>2022-12-10</t>
-  </si>
-  <si>
-    <t>2023-01-10</t>
-  </si>
-  <si>
-    <t>2023-01-18</t>
-  </si>
-  <si>
-    <t>2023-02-10</t>
-  </si>
-  <si>
-    <t>2023-02-12</t>
-  </si>
-  <si>
-    <t>2023-04-02</t>
-  </si>
-  <si>
-    <t>2023-04-10</t>
-  </si>
-  <si>
-    <t>2023-05-10</t>
-  </si>
-  <si>
-    <t>2023-06-02</t>
-  </si>
-  <si>
-    <t>2023-06-10</t>
-  </si>
-  <si>
-    <t>2023-06-26</t>
-  </si>
-  <si>
-    <t>2023-07-10</t>
-  </si>
-  <si>
-    <t>2023-08-10</t>
-  </si>
-  <si>
-    <t>2023-08-15</t>
-  </si>
-  <si>
-    <t>2023-09-10</t>
-  </si>
-  <si>
-    <t>2023-10-10</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-11-20</t>
-  </si>
-  <si>
-    <t>2023-11-24</t>
-  </si>
-  <si>
-    <t>2023-12-24</t>
-  </si>
-  <si>
-    <t>2024-01-10</t>
-  </si>
-  <si>
-    <t>2024-02-10</t>
-  </si>
-  <si>
-    <t>2024-03-10</t>
-  </si>
-  <si>
-    <t>2024-04-10</t>
-  </si>
-  <si>
-    <t>2024-05-10</t>
-  </si>
-  <si>
-    <t>2024-06-10</t>
-  </si>
-  <si>
-    <t>2024-07-10</t>
-  </si>
-  <si>
-    <t>2024-08-10</t>
-  </si>
-  <si>
-    <t>2024-10-10</t>
-  </si>
-  <si>
-    <t>2025-01-10</t>
-  </si>
-  <si>
-    <t>2025-02-10</t>
-  </si>
-  <si>
-    <t>2025-03-10</t>
-  </si>
-  <si>
-    <t>2025-04-10</t>
-  </si>
-  <si>
-    <t>2025-05-10</t>
-  </si>
-  <si>
-    <t>2025-06-10</t>
-  </si>
-  <si>
-    <t>2025-07-10</t>
-  </si>
-  <si>
-    <t>2025-08-10</t>
-  </si>
-  <si>
-    <t>2025-10-10</t>
-  </si>
-  <si>
-    <t>2026-01-10</t>
-  </si>
-  <si>
-    <t>2026-03-10</t>
-  </si>
-  <si>
-    <t>2027-01-10</t>
-  </si>
-  <si>
-    <t>2027-02-10</t>
-  </si>
-  <si>
-    <t>2028-07-10</t>
+    <t>2011-03-03</t>
+  </si>
+  <si>
+    <t>2011-06-03</t>
+  </si>
+  <si>
+    <t>2011-07-03</t>
+  </si>
+  <si>
+    <t>2011-12-03</t>
+  </si>
+  <si>
+    <t>2014-09-03</t>
+  </si>
+  <si>
+    <t>2014-10-03</t>
+  </si>
+  <si>
+    <t>2014-11-03</t>
+  </si>
+  <si>
+    <t>2014-12-03</t>
+  </si>
+  <si>
+    <t>2015-03-03</t>
+  </si>
+  <si>
+    <t>2016-01-03</t>
+  </si>
+  <si>
+    <t>2016-04-03</t>
+  </si>
+  <si>
+    <t>2016-08-03</t>
+  </si>
+  <si>
+    <t>2017-01-03</t>
+  </si>
+  <si>
+    <t>2017-08-03</t>
+  </si>
+  <si>
+    <t>2017-09-03</t>
+  </si>
+  <si>
+    <t>2017-10-03</t>
+  </si>
+  <si>
+    <t>2017-11-03</t>
+  </si>
+  <si>
+    <t>2018-05-03</t>
+  </si>
+  <si>
+    <t>2018-07-03</t>
+  </si>
+  <si>
+    <t>2019-05-03</t>
+  </si>
+  <si>
+    <t>2019-06-03</t>
+  </si>
+  <si>
+    <t>2019-08-03</t>
+  </si>
+  <si>
+    <t>2019-09-03</t>
+  </si>
+  <si>
+    <t>2020-01-03</t>
+  </si>
+  <si>
+    <t>2020-03-03</t>
+  </si>
+  <si>
+    <t>2020-04-03</t>
+  </si>
+  <si>
+    <t>2020-05-03</t>
+  </si>
+  <si>
+    <t>2020-07-03</t>
+  </si>
+  <si>
+    <t>2020-08-03</t>
+  </si>
+  <si>
+    <t>2020-11-03</t>
+  </si>
+  <si>
+    <t>2021-02-03</t>
+  </si>
+  <si>
+    <t>2021-05-03</t>
+  </si>
+  <si>
+    <t>2021-06-03</t>
+  </si>
+  <si>
+    <t>2021-09-03</t>
+  </si>
+  <si>
+    <t>2021-12-03</t>
+  </si>
+  <si>
+    <t>2022-01-03</t>
+  </si>
+  <si>
+    <t>2022-03-03</t>
+  </si>
+  <si>
+    <t>2022-04-03</t>
+  </si>
+  <si>
+    <t>2022-05-03</t>
+  </si>
+  <si>
+    <t>2022-06-03</t>
+  </si>
+  <si>
+    <t>2022-07-03</t>
+  </si>
+  <si>
+    <t>2022-08-03</t>
+  </si>
+  <si>
+    <t>2022-09-03</t>
+  </si>
+  <si>
+    <t>2022-10-03</t>
+  </si>
+  <si>
+    <t>2022-11-03</t>
+  </si>
+  <si>
+    <t>2022-12-03</t>
+  </si>
+  <si>
+    <t>2023-01-03</t>
+  </si>
+  <si>
+    <t>2023-02-03</t>
+  </si>
+  <si>
+    <t>2023-04-03</t>
+  </si>
+  <si>
+    <t>2023-05-03</t>
+  </si>
+  <si>
+    <t>2023-06-03</t>
+  </si>
+  <si>
+    <t>2023-07-03</t>
+  </si>
+  <si>
+    <t>2023-08-03</t>
+  </si>
+  <si>
+    <t>2023-09-03</t>
+  </si>
+  <si>
+    <t>2023-10-03</t>
+  </si>
+  <si>
+    <t>2024-01-03</t>
+  </si>
+  <si>
+    <t>2024-01-18</t>
+  </si>
+  <si>
+    <t>2024-02-03</t>
+  </si>
+  <si>
+    <t>2024-02-12</t>
+  </si>
+  <si>
+    <t>2024-03-03</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
+  </si>
+  <si>
+    <t>2024-04-03</t>
+  </si>
+  <si>
+    <t>2024-05-03</t>
+  </si>
+  <si>
+    <t>2024-06-02</t>
+  </si>
+  <si>
+    <t>2024-06-03</t>
+  </si>
+  <si>
+    <t>2024-06-26</t>
+  </si>
+  <si>
+    <t>2024-07-03</t>
+  </si>
+  <si>
+    <t>2024-08-03</t>
+  </si>
+  <si>
+    <t>2024-08-15</t>
+  </si>
+  <si>
+    <t>2024-10-03</t>
+  </si>
+  <si>
+    <t>2024-10-24</t>
+  </si>
+  <si>
+    <t>2024-11-20</t>
+  </si>
+  <si>
+    <t>2024-11-24</t>
+  </si>
+  <si>
+    <t>2024-12-24</t>
+  </si>
+  <si>
+    <t>2025-01-03</t>
+  </si>
+  <si>
+    <t>2025-02-03</t>
+  </si>
+  <si>
+    <t>2025-03-03</t>
+  </si>
+  <si>
+    <t>2025-04-03</t>
+  </si>
+  <si>
+    <t>2025-05-03</t>
+  </si>
+  <si>
+    <t>2025-06-03</t>
+  </si>
+  <si>
+    <t>2025-07-03</t>
+  </si>
+  <si>
+    <t>2025-08-03</t>
+  </si>
+  <si>
+    <t>2025-10-03</t>
+  </si>
+  <si>
+    <t>2026-01-03</t>
+  </si>
+  <si>
+    <t>2026-03-03</t>
+  </si>
+  <si>
+    <t>2027-01-03</t>
+  </si>
+  <si>
+    <t>2027-02-03</t>
+  </si>
+  <si>
+    <t>2028-07-03</t>
   </si>
 </sst>
 </file>
@@ -1818,7 +1818,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1834,7 +1834,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1842,7 +1842,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1850,7 +1850,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1858,7 +1858,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1866,7 +1866,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1874,7 +1874,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1882,7 +1882,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1890,7 +1890,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1898,7 +1898,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1906,7 +1906,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1914,7 +1914,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1922,7 +1922,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1930,7 +1930,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1938,7 +1938,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1946,7 +1946,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1954,7 +1954,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1986,7 +1986,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2010,7 +2010,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2018,7 +2018,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2026,7 +2026,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2034,7 +2034,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2042,7 +2042,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2050,7 +2050,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2090,7 +2090,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2098,7 +2098,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2106,7 +2106,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2114,7 +2114,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2130,7 +2130,7 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2154,7 +2154,7 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2170,7 +2170,7 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2178,7 +2178,7 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2186,7 +2186,7 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2242,7 +2242,7 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2274,7 +2274,7 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2298,7 +2298,7 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2306,7 +2306,7 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2322,7 +2322,7 @@
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2338,7 +2338,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="146" spans="1:2">

</xml_diff>

<commit_message>
remove posixpath from Link generation in changes files make "review dates" optional in build
</commit_message>
<xml_diff>
--- a/lothiancriticalcare/1a74f8f7b8b7e871b413c4697f68b4401fbacdf0/reviewdates.xlsx
+++ b/lothiancriticalcare/1a74f8f7b8b7e871b413c4697f68b4401fbacdf0/reviewdates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="281">
   <si>
     <t>File</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Drugs/heparin_critical_care_only.pdf</t>
   </si>
   <si>
-    <t>Routine_Care/test_20240309.pdf</t>
-  </si>
-  <si>
     <t>Routine_Care/Invasive Flush Systems.pdf</t>
   </si>
   <si>
@@ -88,15 +85,15 @@
     <t>End_of_life_care/Reasons to report a death to PF.pdf</t>
   </si>
   <si>
+    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy change in Critical Care.pdf</t>
+  </si>
+  <si>
     <t>Neurological/SOP -  Femoral site care.pdf</t>
   </si>
   <si>
     <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy suctioning cleaning guideline.pdf</t>
   </si>
   <si>
-    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy change in Critical Care.pdf</t>
-  </si>
-  <si>
     <t>Drugs/sodium_bicarbonate.pdf</t>
   </si>
   <si>
@@ -106,24 +103,24 @@
     <t>Post_op_care/Epidural top-up.pdf</t>
   </si>
   <si>
+    <t>Covid-19/SJH/SJH COVID19 ED Intubation Action Card.pdf</t>
+  </si>
+  <si>
+    <t>Covid-19/SJH/SJH COVID19 ITU Intubation Action Card.pdf</t>
+  </si>
+  <si>
+    <t>Airway/Emergency intubation checklist_em_pub.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/heparin for Haemofiltration.pdf</t>
+  </si>
+  <si>
+    <t>Diabetes_and_Glucose/Hyperosmolar Hyperglycaemic State.pdf</t>
+  </si>
+  <si>
     <t>Covid-19/WGH/CoVid intubation checklist WGH.pdf</t>
   </si>
   <si>
-    <t>Covid-19/SJH/SJH COVID19 ITU Intubation Action Card.pdf</t>
-  </si>
-  <si>
-    <t>Covid-19/SJH/SJH COVID19 ED Intubation Action Card.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/heparin for Haemofiltration.pdf</t>
-  </si>
-  <si>
-    <t>Diabetes_and_Glucose/Hyperosmolar Hyperglycaemic State.pdf</t>
-  </si>
-  <si>
-    <t>Airway/Emergency intubation checklist_em_pub.pdf</t>
-  </si>
-  <si>
     <t>Drugs/fentanyl.pdf</t>
   </si>
   <si>
@@ -142,42 +139,42 @@
     <t>Airway/Percutaneous tracheostomy checklist.pdf</t>
   </si>
   <si>
+    <t>Delirium/Risk assessment posi mit.pdf</t>
+  </si>
+  <si>
+    <t>Infection_and_sepsis/SOP Ultrasound Cleaning.pdf</t>
+  </si>
+  <si>
     <t>Delirium/Managing a Potentially Violent Patient.pdf</t>
   </si>
   <si>
-    <t>Delirium/Risk assessment posi mit.pdf</t>
-  </si>
-  <si>
-    <t>Infection_and_sepsis/SOP Ultrasound Cleaning.pdf</t>
+    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy safety box contents.pdf</t>
+  </si>
+  <si>
+    <t>Neurological/Sub arachnoid haemorrhage management.pdf</t>
+  </si>
+  <si>
+    <t>Breathing(Respiratory)/HFNO.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/ketamine_in_asthma.pdf</t>
+  </si>
+  <si>
+    <t>Airway/Anticipated difficult airway tool.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/Abdominal pressure measurement.pdf</t>
   </si>
   <si>
     <t>GI_Liver_and_Transplant/Treatment of constipation.pdf</t>
   </si>
   <si>
-    <t>GI_Liver_and_Transplant/Abdominal pressure measurement.pdf</t>
-  </si>
-  <si>
-    <t>Airway/Anticipated difficult airway tool.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/ketamine_in_asthma.pdf</t>
-  </si>
-  <si>
-    <t>Breathing(Respiratory)/HFNO.pdf</t>
-  </si>
-  <si>
     <t>Airway/McGrath Mac.pdf</t>
   </si>
   <si>
-    <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy safety box contents.pdf</t>
-  </si>
-  <si>
     <t>Delirium/Drugs Causing Delirium and Agitiation.pdf</t>
   </si>
   <si>
-    <t>Neurological/Sub arachnoid haemorrhage management.pdf</t>
-  </si>
-  <si>
     <t>End_of_life_care/Documentation following death.pdf</t>
   </si>
   <si>
@@ -187,12 +184,12 @@
     <t>Routine_Care/bBraun Spaceplus Failure EMERGENCY ACTION CARD_em.pdf</t>
   </si>
   <si>
+    <t>Breathing(Respiratory)/Equipment/HFNO Set Up.pdf</t>
+  </si>
+  <si>
     <t>Drugs/insulin.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/Equipment/HFNO Set Up.pdf</t>
-  </si>
-  <si>
     <t>Breathing(Respiratory)/Inhaled Nitrous Oxide.pdf</t>
   </si>
   <si>
@@ -202,15 +199,15 @@
     <t>Breathing(Respiratory)/Equipment/APRV.pdf</t>
   </si>
   <si>
+    <t>Breathing(Respiratory)/Equipment/T piece Y piece.pdf</t>
+  </si>
+  <si>
     <t>Post_op_care/Epidural Haematoma.pdf</t>
   </si>
   <si>
     <t>Neurological/SOP for review of Neurosurgical patients in ITU by neurosurgical team.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/Equipment/T piece Y piece.pdf</t>
-  </si>
-  <si>
     <t>Policies_and_admin/General Critical Care Interaction with HEPMA_pub.pdf</t>
   </si>
   <si>
@@ -220,24 +217,24 @@
     <t>Breathing(Respiratory)/Equipment/HFNO through ventilator.pdf</t>
   </si>
   <si>
+    <t>Post_op_care/Adult Scoliosis Spinal Surgery Post-Op Care.pdf</t>
+  </si>
+  <si>
     <t>Routine_Care/VTE_Prevention/Dalteparin_thromboprophylaxis.pdf</t>
   </si>
   <si>
-    <t>Post_op_care/Adult Scoliosis Spinal Surgery Post-Op Care.pdf</t>
-  </si>
-  <si>
     <t>Post_op_care/Post op care pharyngo-laryngo-oesphagectomy PLOG.pdf</t>
   </si>
   <si>
     <t>GI_Liver_and_Transplant/Nasogastric feeding protocol.pdf</t>
   </si>
   <si>
+    <t>Diabetes_and_Glucose/Intravenous Insulin Therapy (not for DKA or HHS).pdf</t>
+  </si>
+  <si>
     <t>Drugs/Antibiotic doses in CVVHD.pdf</t>
   </si>
   <si>
-    <t>Diabetes_and_Glucose/Intravenous Insulin Therapy (not for DKA or HHS).pdf</t>
-  </si>
-  <si>
     <t>GI_Liver_and_Transplant/Nasojejunal feeding protocol.pdf</t>
   </si>
   <si>
@@ -247,54 +244,54 @@
     <t>ECLS/RIE ECLS Anti Xa Protocol.pdf</t>
   </si>
   <si>
+    <t>Drugs/vasopressin_sepsis.pdf</t>
+  </si>
+  <si>
     <t>Infection_and_sepsis/Winter Infections Stepdown Guidance.pdf</t>
   </si>
   <si>
-    <t>Drugs/vasopressin_sepsis.pdf</t>
-  </si>
-  <si>
     <t>Drugs/vasopressin organ donation.pdf</t>
   </si>
   <si>
+    <t>Transfer/ACCP Transfers.pdf</t>
+  </si>
+  <si>
     <t>Covid-19/videos/Donning and Doffing Video.pdf</t>
   </si>
   <si>
-    <t>Transfer/ACCP Transfers.pdf</t>
+    <t>Drugs/piperacillin_tazobactam extended_infusion.pdf</t>
+  </si>
+  <si>
+    <t>Infection_and_sepsis/Infection indications for IVIG.pdf</t>
   </si>
   <si>
     <t>Breathing(Respiratory)/Equipment/Bipap V60.pdf</t>
   </si>
   <si>
+    <t>Breathing(Respiratory)/Equipment/Ventilators Circuits Filters and Closed Suction - Set up and Maintenance.pdf</t>
+  </si>
+  <si>
     <t>Breathing(Respiratory)/CPAP.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/Equipment/Ventilators Circuits Filters and Closed Suction - Set up and Maintenance.pdf</t>
-  </si>
-  <si>
-    <t>Infection_and_sepsis/Infection indications for IVIG.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/piperacillin_tazobactam extended_infusion.pdf</t>
-  </si>
-  <si>
     <t>Procedures/CVC Guidance/Securing CVCs.pdf</t>
   </si>
   <si>
     <t>Covid-19/Covid 19 Death Certification Guideline.pdf</t>
   </si>
   <si>
+    <t>Routine_Care/Video Communication.pdf</t>
+  </si>
+  <si>
     <t>Neurological/Treatment of status epilepticus.pdf</t>
   </si>
   <si>
-    <t>Routine_Care/Video Communication.pdf</t>
+    <t>Drugs/isoprenaline.pdf</t>
   </si>
   <si>
     <t>Cardiovascular/Cardiogenic Shock.pdf</t>
   </si>
   <si>
-    <t>Drugs/isoprenaline.pdf</t>
-  </si>
-  <si>
     <t>Haematology_CAR-T/Haem_ICU_transfer.pdf</t>
   </si>
   <si>
@@ -304,18 +301,18 @@
     <t>Cardiovascular/Management of hypertension within Critical Care.pdf</t>
   </si>
   <si>
+    <t>Haematology_CAR-T/CRS.pdf</t>
+  </si>
+  <si>
     <t>Drugs/phenytoin.pdf</t>
   </si>
   <si>
+    <t>Drugs/pancuronium.pdf</t>
+  </si>
+  <si>
     <t>Haematology_CAR-T/ICANS.pdf</t>
   </si>
   <si>
-    <t>Drugs/pancuronium.pdf</t>
-  </si>
-  <si>
-    <t>Haematology_CAR-T/CRS.pdf</t>
-  </si>
-  <si>
     <t>Drugs/rocuronium.pdf</t>
   </si>
   <si>
@@ -325,39 +322,39 @@
     <t>Policies_and_admin/General Critical Care SOP_pub.pdf</t>
   </si>
   <si>
+    <t>Covid-19/COVID 19 ICM guidance basic goals_June_2022.pdf</t>
+  </si>
+  <si>
+    <t>Organ_donation/Organ Retrieval SOP.pdf</t>
+  </si>
+  <si>
+    <t>Neurological/Management of traumatic brain injury.pdf</t>
+  </si>
+  <si>
+    <t>Ethics_and_Law/Care at the End of Life (FICM).pdf</t>
+  </si>
+  <si>
+    <t>Ethics_and_Law/DNACPR policy for Scotland.pdf</t>
+  </si>
+  <si>
+    <t>End_of_life_care/Palliative extubation &amp; withdrawal of invasive ventilatory support nursing checklist.pdf</t>
+  </si>
+  <si>
+    <t>Neurological/Critical Care MRI Procedure_pub.pdf</t>
+  </si>
+  <si>
+    <t>Infection_and_sepsis/Trip Out of Unit infection guidance.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/ICU - Upper GI bleeding (Endoscopy guideline).pdf</t>
+  </si>
+  <si>
     <t>Drugs/clonidine.pdf</t>
   </si>
   <si>
-    <t>Organ_donation/Organ Retrieval SOP.pdf</t>
-  </si>
-  <si>
-    <t>End_of_life_care/Palliative extubation &amp; withdrawal of invasive ventilatory support nursing checklist.pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/ICU - Upper GI bleeding (Endoscopy guideline).pdf</t>
-  </si>
-  <si>
-    <t>Neurological/Critical Care MRI Procedure_pub.pdf</t>
-  </si>
-  <si>
-    <t>Ethics_and_Law/DNACPR policy for Scotland.pdf</t>
-  </si>
-  <si>
-    <t>Ethics_and_Law/Care at the End of Life (FICM).pdf</t>
-  </si>
-  <si>
     <t>End_of_life_care/CMO &amp; NRS Guidance for Doctors completing MCCD.pdf</t>
   </si>
   <si>
-    <t>Neurological/Management of traumatic brain injury.pdf</t>
-  </si>
-  <si>
-    <t>Infection_and_sepsis/Trip Out of Unit infection guidance.pdf</t>
-  </si>
-  <si>
-    <t>Covid-19/COVID 19 ICM guidance basic goals_June_2022.pdf</t>
-  </si>
-  <si>
     <t>Airway/Cook Staged Extubation Set.pdf</t>
   </si>
   <si>
@@ -367,21 +364,21 @@
     <t>Post_op_care/Epidural hypotension.pdf</t>
   </si>
   <si>
+    <t>Drugs/glyceryl_trinitrate.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/Confirmation of Nasogastric Tube Position.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/dexmedetomidine.pdf</t>
+  </si>
+  <si>
+    <t>Breathing(Respiratory)/Equipment/Passy Muir Valve.pdf</t>
+  </si>
+  <si>
     <t>GI_Liver_and_Transplant/Fulminant Liver Failure.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/Equipment/Passy Muir Valve.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/glyceryl_trinitrate.pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/Confirmation of Nasogastric Tube Position.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/dexmedetomidine.pdf</t>
-  </si>
-  <si>
     <t>Infection_and_sepsis/Antifungal guidance in critical care.pdf</t>
   </si>
   <si>
@@ -397,24 +394,24 @@
     <t>Breathing(Respiratory)/ARDS Strategy.pdf</t>
   </si>
   <si>
+    <t>Drugs/adrenaline.pdf</t>
+  </si>
+  <si>
     <t>Drugs/dobutamine.pdf</t>
   </si>
   <si>
-    <t>Drugs/adrenaline.pdf</t>
-  </si>
-  <si>
     <t>Drugs/hydralazine.pdf</t>
   </si>
   <si>
     <t>Post_op_care/Major OMFS Free Flap.pdf</t>
   </si>
   <si>
+    <t>Drugs/Alteplase for massive PE.pdf</t>
+  </si>
+  <si>
     <t>Drugs/alfentanil.pdf</t>
   </si>
   <si>
-    <t>Drugs/Alteplase for massive PE.pdf</t>
-  </si>
-  <si>
     <t>Drugs/magnesium.pdf</t>
   </si>
   <si>
@@ -427,31 +424,43 @@
     <t>Drugs/vancomycin.pdf</t>
   </si>
   <si>
+    <t>Infection_and_sepsis/Initial investigation and management in unidentified Infections.pdf</t>
+  </si>
+  <si>
+    <t>Neurological/Intrathecal policy RIE.pdf</t>
+  </si>
+  <si>
     <t>Drugs/labetalol.pdf</t>
   </si>
   <si>
-    <t>Neurological/Intrathecal policy RIE.pdf</t>
-  </si>
-  <si>
-    <t>Infection_and_sepsis/Initial investigation and management in unidentified Infections.pdf</t>
+    <t>Cardiovascular/Management of Acute Type B Aortic Dissection Guideline.pdf</t>
   </si>
   <si>
     <t>Drugs/midazolam.pdf</t>
   </si>
   <si>
-    <t>Cardiovascular/Management of Acute Type B Aortic Dissection Guideline.pdf</t>
+    <t>Procedures/CVC Guidance/CVC NHL  April 2023.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/potassium.pdf</t>
   </si>
   <si>
     <t>Drugs/salbutamol.pdf</t>
   </si>
   <si>
-    <t>Procedures/CVC Guidance/CVC NHL  April 2023.pdf</t>
-  </si>
-  <si>
     <t>Drugs/nimodipine.pdf</t>
   </si>
   <si>
-    <t>Drugs/potassium.pdf</t>
+    <t>Procedures/Arterial Line insertion for ACCPs.pdf</t>
+  </si>
+  <si>
+    <t>Routine_Care/newtest_c.pdf</t>
+  </si>
+  <si>
+    <t>Routine_Care/newtest_c copy.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/nicardipine.pdf</t>
   </si>
   <si>
     <t>Drugs/phenobarbitone.pdf</t>
@@ -460,40 +469,40 @@
     <t>Routine_Care/ICU Eye Care Guideline.pdf</t>
   </si>
   <si>
-    <t>Drugs/nicardipine.pdf</t>
-  </si>
-  <si>
     <t>Drugs/amiodarone.pdf</t>
   </si>
   <si>
-    <t>Procedures/Arterial Line insertion for ACCPs.pdf</t>
+    <t>Drugs/morphine.pdf</t>
   </si>
   <si>
     <t>Drugs/noradrenaline (peripheral).pdf</t>
   </si>
   <si>
+    <t>Neurological/Ventriculitis Guideline.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/phenylephrine.pdf</t>
+  </si>
+  <si>
     <t>Drugs/Epoprostenol.pdf</t>
   </si>
   <si>
     <t>Breathing(Respiratory)/Manual Ventilation and MHI.pdf</t>
   </si>
   <si>
-    <t>Neurological/Ventriculitis Guideline.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/phenylephrine.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/morphine.pdf</t>
+    <t>Drugs/calcium.pdf</t>
+  </si>
+  <si>
+    <t>Cardiovascular/Pulmonary_Embolism_and_DVT/Catheter directed thrombolysis of iliofemoral DVT alteplase_pub.pdf</t>
   </si>
   <si>
     <t>Cardiovascular/Cardiac Output Monitoring_pub .pdf</t>
   </si>
   <si>
-    <t>Cardiovascular/Pulmonary_Embolism_and_DVT/Catheter directed thrombolysis of iliofemoral DVT alteplase_pub.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/calcium.pdf</t>
+    <t>Airway/Tracheostomy_Laryngectomy/Decannulation Guidline.pdf</t>
+  </si>
+  <si>
+    <t>Drugs/atracurium.pdf</t>
   </si>
   <si>
     <t>Drugs/dalteparin_thromboprophylaxis.pdf</t>
@@ -502,10 +511,7 @@
     <t>Drugs/Vancomycin Continuous Infusion Fluid Restricted.pdf</t>
   </si>
   <si>
-    <t>Drugs/atracurium.pdf</t>
-  </si>
-  <si>
-    <t>Airway/Tracheostomy_Laryngectomy/Decannulation Guidline.pdf</t>
+    <t>Procedures/Inadvertent Catheter Placement Guideline.pdf</t>
   </si>
   <si>
     <t>Policies_and_admin/Pet Visitation.pdf</t>
@@ -514,7 +520,7 @@
     <t>Drugs/valproate.pdf</t>
   </si>
   <si>
-    <t>Procedures/Inadvertent Catheter Placement Guideline.pdf</t>
+    <t>Drugs/Phosphate.pdf</t>
   </si>
   <si>
     <t>Drugs/stress ulcer prophylaxis.pdf</t>
@@ -523,30 +529,27 @@
     <t>Drugs/ketamine_for_status epilepticus.pdf</t>
   </si>
   <si>
-    <t>Drugs/Phosphate.pdf</t>
+    <t>Drugs/Octreotide.pdf</t>
+  </si>
+  <si>
+    <t>Breathing(Respiratory)/Proning Guideline.pdf</t>
+  </si>
+  <si>
+    <t>GI_Liver_and_Transplant/Prokinetics in ICU.pdf</t>
   </si>
   <si>
     <t>Drugs/Thiopentone.pdf</t>
   </si>
   <si>
-    <t>Breathing(Respiratory)/Proning Guideline.pdf</t>
-  </si>
-  <si>
-    <t>GI_Liver_and_Transplant/Prokinetics in ICU.pdf</t>
-  </si>
-  <si>
-    <t>Drugs/Octreotide.pdf</t>
-  </si>
-  <si>
     <t>Procedures/ACCP CVC placement following completion of initial competencies.pdf</t>
   </si>
   <si>
+    <t>Post_op_care/Prevention and treatment of paraplegia after major aortic procedures.pdf</t>
+  </si>
+  <si>
     <t>Procedures/ACCPs acquiring initial CVC competencies.pdf</t>
   </si>
   <si>
-    <t>Post_op_care/Prevention and treatment of paraplegia after major aortic procedures.pdf</t>
-  </si>
-  <si>
     <t>Delirium/Violence and Agression.pdf</t>
   </si>
   <si>
@@ -556,10 +559,10 @@
     <t>GI_Liver_and_Transplant/Plasma exchange in Acute Liver Failure.pdf</t>
   </si>
   <si>
+    <t>Breathing(Respiratory)/Equipment/NIV through Drager Vent Set up in Critical Care.pdf</t>
+  </si>
+  <si>
     <t>End_of_life_care/Guideline following Sudden Cardiac Death where death occurs in ICU.pdf</t>
-  </si>
-  <si>
-    <t>Breathing(Respiratory)/Equipment/NIV through Drager Vent Set up in Critical Care.pdf</t>
   </si>
   <si>
     <t>Transfer/Transfer Guidelines.pdf</t>
@@ -1211,7 +1214,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1230,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1238,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1246,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1254,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1262,7 +1265,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1270,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1278,7 +1281,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1286,7 +1289,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1294,7 +1297,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1302,7 +1305,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1310,7 +1313,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1318,7 +1321,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1326,7 +1329,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1334,7 +1337,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1342,7 +1345,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1350,7 +1353,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1358,7 +1361,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1366,7 +1369,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1374,7 +1377,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1382,7 +1385,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1390,7 +1393,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1398,7 +1401,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1406,7 +1409,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1414,7 +1417,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1422,7 +1425,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1430,7 +1433,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1438,7 +1441,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1446,7 +1449,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1454,7 +1457,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1462,7 +1465,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1470,7 +1473,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1478,7 +1481,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1486,7 +1489,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1494,7 +1497,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1502,7 +1505,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1510,7 +1513,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1518,7 +1521,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1526,7 +1529,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1534,7 +1537,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1542,7 +1545,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1550,7 +1553,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1558,7 +1561,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1566,7 +1569,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1574,7 +1577,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1582,7 +1585,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1590,7 +1593,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1598,7 +1601,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1606,7 +1609,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1614,7 +1617,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1622,7 +1625,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1630,7 +1633,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1638,7 +1641,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1646,7 +1649,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1654,7 +1657,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1662,7 +1665,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1670,7 +1673,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1678,7 +1681,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1686,7 +1689,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1694,7 +1697,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1702,7 +1705,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1710,7 +1713,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1718,7 +1721,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1726,7 +1729,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1734,7 +1737,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1742,7 +1745,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1750,7 +1753,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1758,7 +1761,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1766,7 +1769,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1774,7 +1777,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1782,7 +1785,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1790,7 +1793,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1798,7 +1801,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1806,7 +1809,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1814,7 +1817,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1822,7 +1825,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1830,7 +1833,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1838,7 +1841,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1846,7 +1849,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1854,7 +1857,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1862,7 +1865,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1870,7 +1873,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1878,7 +1881,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1886,7 +1889,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1894,7 +1897,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1902,7 +1905,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1910,7 +1913,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1918,7 +1921,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1926,7 +1929,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1934,7 +1937,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1942,7 +1945,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1950,7 +1953,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1958,7 +1961,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1966,7 +1969,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1974,7 +1977,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1982,7 +1985,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1990,7 +1993,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1998,7 +2001,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2006,7 +2009,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2014,7 +2017,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2022,7 +2025,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2030,7 +2033,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2038,7 +2041,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2046,7 +2049,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2054,7 +2057,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2062,7 +2065,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2070,7 +2073,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2078,7 +2081,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2086,7 +2089,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2094,7 +2097,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2102,7 +2105,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2110,7 +2113,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2118,7 +2121,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2126,7 +2129,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2134,7 +2137,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2142,7 +2145,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2150,7 +2153,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2158,7 +2161,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2166,7 +2169,7 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2174,7 +2177,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2182,7 +2185,7 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2190,7 +2193,7 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2198,7 +2201,7 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2206,7 +2209,7 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2214,7 +2217,7 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2222,7 +2225,7 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2230,7 +2233,7 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2238,7 +2241,7 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2246,7 +2249,7 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2254,7 +2257,7 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2262,7 +2265,7 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2270,7 +2273,7 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2278,7 +2281,7 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2286,7 +2289,7 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2294,7 +2297,7 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2302,7 +2305,7 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2310,7 +2313,7 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2318,7 +2321,7 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2326,7 +2329,7 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2334,7 +2337,7 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2342,7 +2345,7 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2350,7 +2353,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2358,7 +2361,7 @@
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2366,7 +2369,7 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2374,7 +2377,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2382,7 +2385,7 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2390,7 +2393,7 @@
         <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2398,7 +2401,7 @@
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2406,7 +2409,7 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2414,7 +2417,7 @@
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2430,7 +2433,7 @@
         <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2438,7 +2441,7 @@
         <v>153</v>
       </c>
       <c r="B153" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2446,7 +2449,7 @@
         <v>154</v>
       </c>
       <c r="B154" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2454,7 +2457,7 @@
         <v>155</v>
       </c>
       <c r="B155" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2462,7 +2465,7 @@
         <v>156</v>
       </c>
       <c r="B156" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2478,7 +2481,7 @@
         <v>158</v>
       </c>
       <c r="B158" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2486,7 +2489,7 @@
         <v>159</v>
       </c>
       <c r="B159" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2502,7 +2505,7 @@
         <v>161</v>
       </c>
       <c r="B161" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2510,7 +2513,7 @@
         <v>162</v>
       </c>
       <c r="B162" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2518,7 +2521,7 @@
         <v>163</v>
       </c>
       <c r="B163" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2534,7 +2537,7 @@
         <v>165</v>
       </c>
       <c r="B165" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2542,7 +2545,7 @@
         <v>166</v>
       </c>
       <c r="B166" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2558,7 +2561,7 @@
         <v>168</v>
       </c>
       <c r="B168" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2566,7 +2569,7 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2582,7 +2585,7 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2590,7 +2593,7 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2598,7 +2601,7 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2614,7 +2617,7 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2622,7 +2625,7 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2662,7 +2665,7 @@
         <v>181</v>
       </c>
       <c r="B181" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2711,6 +2714,14 @@
       </c>
       <c r="B187" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>188</v>
+      </c>
+      <c r="B188" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>